<commit_message>
Added more Search test steps
</commit_message>
<xml_diff>
--- a/TGLAutomation/src/test/resources/testdata/MasterSheet.xlsx
+++ b/TGLAutomation/src/test/resources/testdata/MasterSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitin.sharma\Workspace2\TGLAutomation\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Local_Rep\TGL-Automation\tgl-selenium-automation\TGLAutomation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Locators!$A$1:$A$3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="133">
   <si>
     <t>S.N.</t>
   </si>
@@ -412,6 +411,24 @@
   </si>
   <si>
     <t>Tgl_personid</t>
+  </si>
+  <si>
+    <t>(//div[@class='selectize-input items not-full has-options']/input)[1]</t>
+  </si>
+  <si>
+    <t>Tgl_InterviewDeadlinefilter_txt</t>
+  </si>
+  <si>
+    <t>(//div[@class='selectize-input items not-full has-options']/input)[2]</t>
+  </si>
+  <si>
+    <t>(//div[@class='selectize-input items not-full has-options']/input)[3]</t>
+  </si>
+  <si>
+    <t>Tgl_TGLStatus_txt</t>
+  </si>
+  <si>
+    <t>Tgl_OfferDeadline_txt</t>
   </si>
 </sst>
 </file>
@@ -1254,8 +1271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1779,25 +1796,55 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="21"/>
+      <c r="A30" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="21"/>
+      <c r="A31" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="21"/>
+      <c r="A32" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="20"/>

</xml_diff>

<commit_message>
Search Module Tests complete.
Since this is a complex test which required lot of maneuvering with
locators hence they are hardcoded in the Page Class - SearchPageTGL.java
until some better mechanism is thought of.
</commit_message>
<xml_diff>
--- a/TGLAutomation/src/test/resources/testdata/MasterSheet.xlsx
+++ b/TGLAutomation/src/test/resources/testdata/MasterSheet.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="133">
   <si>
     <t>S.N.</t>
   </si>
@@ -395,15 +395,6 @@
     <t>Tgl_offerdeadlineInput_dd</t>
   </si>
   <si>
-    <t>#firstname-input</t>
-  </si>
-  <si>
-    <t>#personid-input</t>
-  </si>
-  <si>
-    <t>#lastname-input</t>
-  </si>
-  <si>
     <t>Tgl_firstname</t>
   </si>
   <si>
@@ -419,16 +410,25 @@
     <t>Tgl_InterviewDeadlinefilter_txt</t>
   </si>
   <si>
-    <t>(//div[@class='selectize-input items not-full has-options']/input)[2]</t>
-  </si>
-  <si>
-    <t>(//div[@class='selectize-input items not-full has-options']/input)[3]</t>
-  </si>
-  <si>
     <t>Tgl_TGLStatus_txt</t>
   </si>
   <si>
     <t>Tgl_OfferDeadline_txt</t>
+  </si>
+  <si>
+    <t>//tbody[@data-hook='results']/tr[1]/td/a</t>
+  </si>
+  <si>
+    <t>Tgl_firstrow_name</t>
+  </si>
+  <si>
+    <t>//input[@id='firstname-input']</t>
+  </si>
+  <si>
+    <t>//input[@id='lastname-input']</t>
+  </si>
+  <si>
+    <t>//input[@id='personid-input']</t>
   </si>
 </sst>
 </file>
@@ -1272,7 +1272,7 @@
   <dimension ref="A1:U43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,13 +1752,13 @@
         <v>112</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1769,13 +1769,13 @@
         <v>112</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1786,13 +1786,13 @@
         <v>112</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1803,13 +1803,13 @@
         <v>112</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D30" s="20" t="s">
         <v>88</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1820,13 +1820,13 @@
         <v>112</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D31" s="20" t="s">
         <v>88</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1837,21 +1837,31 @@
         <v>112</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D32" s="20" t="s">
         <v>88</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="20"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="21"/>
+      <c r="A33" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="21" t="s">
+        <v>129</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E33" s="21" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="20"/>

</xml_diff>

<commit_message>
Added more code comments
</commit_message>
<xml_diff>
--- a/TGLAutomation/src/test/resources/testdata/MasterSheet.xlsx
+++ b/TGLAutomation/src/test/resources/testdata/MasterSheet.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="250">
   <si>
     <t>S.N.</t>
   </si>
@@ -263,9 +263,6 @@
     <t>https://qamerlin.teachforamerica.org/ada/sign-in</t>
   </si>
   <si>
-    <t>Accounts##CMM_003</t>
-  </si>
-  <si>
     <t>LoginTgl_username_ED</t>
   </si>
   <si>
@@ -635,9 +632,6 @@
     <t>Tgl_TaxInfoCanClaim_lbl</t>
   </si>
   <si>
-    <t>Tgl_TaxInfoDependent_lbl</t>
-  </si>
-  <si>
     <t>Tgl_TaxInfohowmany_lbl</t>
   </si>
   <si>
@@ -653,9 +647,6 @@
     <t>(//div[@class='document-verification-view'])[5]//td[1]</t>
   </si>
   <si>
-    <t>Tgl_TaxInfo_ApplicantsReturn_lbl</t>
-  </si>
-  <si>
     <t>Tgl_Taxinfoincome_txt</t>
   </si>
   <si>
@@ -687,6 +678,108 @@
   </si>
   <si>
     <t>TGL103</t>
+  </si>
+  <si>
+    <t>(//table[@class='verification-table'])[5]//td[1]</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInforAppTaxReturn_lbl</t>
+  </si>
+  <si>
+    <t>(//table[@class='verification-table'])[5]//td[2]/tfa-input</t>
+  </si>
+  <si>
+    <t>(//table[@class='verification-table'])[5]//td[3]/tfa-input</t>
+  </si>
+  <si>
+    <t>(//table[@class='verification-table'])[5]//td[4]/tfa-input</t>
+  </si>
+  <si>
+    <t>(//table[@class='verification-table'])[6]//td[1]</t>
+  </si>
+  <si>
+    <t>(//table[@class='verification-table'])[6]//td[2]/tfa-input</t>
+  </si>
+  <si>
+    <t>(//table[@class='verification-table'])[6]//td[3]/tfa-input</t>
+  </si>
+  <si>
+    <t>(//table[@class='verification-table'])[6]//td[4]/tfa-input</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoIncome_lbl</t>
+  </si>
+  <si>
+    <t>(//table[@class='verification-table'])[7]//td[1]</t>
+  </si>
+  <si>
+    <t>(//table[@class='verification-table'])[7]//td[2]/tfa-input</t>
+  </si>
+  <si>
+    <t>(//table[@class='verification-table'])[7]//td[3]/tfa-input</t>
+  </si>
+  <si>
+    <t>(//table[@class='verification-table'])[7]//td[4]/tfa-input</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInforAppTaxReturnedRequired_chk</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoAppTaxReturnrValid_chk</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoAppTaxReturnAppNotes_txt</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoIncomeRequired_chk</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoIncomeValid_chk</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoIncomeAppNotes_txt</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoParentsTaxReturn_lbl</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoPTRRequired_chk</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoPTRValid_chk</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoPTRAppNotes_txt</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoPISRequired_chk</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoPIS_lbl</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoPISValid_chk</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoPISAppNotes_txt</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfo_ATR_lbl</t>
+  </si>
+  <si>
+    <t>TGL104ValidateTaxlInformationSection</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>TGL104</t>
+  </si>
+  <si>
+    <t>TGLTestData##CMM_003</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoDependentIncome_lbl</t>
   </si>
 </sst>
 </file>
@@ -772,7 +865,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -795,25 +888,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -873,7 +953,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1309,10 +1388,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS5"/>
+  <dimension ref="A1:AS6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1506,16 +1585,16 @@
         <v>2</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>106</v>
-      </c>
-      <c r="C2" s="23" t="s">
-        <v>107</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>59</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>77</v>
+        <v>248</v>
       </c>
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
@@ -1540,58 +1619,75 @@
     </row>
     <row r="3" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="22" t="s">
-        <v>116</v>
-      </c>
       <c r="C3" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>59</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>77</v>
+        <v>248</v>
       </c>
     </row>
     <row r="4" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="B4" s="22" t="s">
-        <v>143</v>
-      </c>
       <c r="C4" s="23" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>59</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>77</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>59</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>77</v>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>247</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>245</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D1048576">
       <formula1>"Y, N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1602,10 +1698,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U73"/>
+  <dimension ref="A1:U89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="E74" sqref="E74"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1697,10 +1793,10 @@
         <v>64</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -1711,13 +1807,13 @@
         <v>7</v>
       </c>
       <c r="C5" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="21" t="s">
         <v>95</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -1728,13 +1824,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>65</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -1745,13 +1841,13 @@
         <v>7</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>65</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -1813,13 +1909,13 @@
         <v>7</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D11" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="21" t="s">
         <v>88</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -1864,24 +1960,24 @@
         <v>72</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="21" t="s">
         <v>88</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D15" s="20" t="s">
         <v>3</v>
@@ -1892,13 +1988,13 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="20" t="s">
         <v>3</v>
@@ -1909,971 +2005,1243 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>81</v>
-      </c>
       <c r="D17" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D18" s="20" t="s">
         <v>65</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C20" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="21" t="s">
         <v>102</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D21" s="20" t="s">
         <v>65</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D23" s="20" t="s">
         <v>65</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B24" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" s="21" t="s">
         <v>112</v>
-      </c>
-      <c r="C24" s="21" t="s">
-        <v>113</v>
       </c>
       <c r="D24" s="20" t="s">
         <v>65</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D25" s="20" t="s">
         <v>65</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E26" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E28" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C29" s="21" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C30" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E30" s="21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C31" s="21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E31" s="21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C33" s="21" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E33" s="21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C35" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C37" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E37" s="21" t="s">
         <v>138</v>
-      </c>
-      <c r="D37" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E37" s="21" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E38" s="21" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E39" s="21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E40" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D41" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D42" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E42" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D43" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D45" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E45" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D46" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E46" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D47" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E47" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D48" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E48" s="21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D49" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E49" s="21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D50" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E50" s="21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D51" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D52" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D53" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E53" s="21" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D55" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C56" s="21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E56" s="21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C57" s="21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D57" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E57" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>185</v>
+        <v>111</v>
+      </c>
+      <c r="C58" s="21" t="s">
+        <v>184</v>
       </c>
       <c r="D58" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E58" s="10" t="s">
-        <v>184</v>
+        <v>87</v>
+      </c>
+      <c r="E58" s="21" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B59" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C59" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E59" s="21" t="s">
         <v>186</v>
-      </c>
-      <c r="D59" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E59" s="10" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>189</v>
+        <v>111</v>
+      </c>
+      <c r="C60" s="21" t="s">
+        <v>188</v>
       </c>
       <c r="D60" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E60" s="10" t="s">
-        <v>188</v>
+        <v>87</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B61" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>191</v>
+        <v>111</v>
+      </c>
+      <c r="C61" s="21" t="s">
+        <v>190</v>
       </c>
       <c r="D61" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E61" s="10" t="s">
-        <v>190</v>
+        <v>87</v>
+      </c>
+      <c r="E61" s="21" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B62" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C62" s="10" t="s">
-        <v>193</v>
+        <v>111</v>
+      </c>
+      <c r="C62" s="21" t="s">
+        <v>192</v>
       </c>
       <c r="D62" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E62" s="10" t="s">
-        <v>192</v>
+        <v>87</v>
+      </c>
+      <c r="E62" s="21" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B63" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C63" s="10" t="s">
-        <v>195</v>
+        <v>111</v>
+      </c>
+      <c r="C63" s="21" t="s">
+        <v>194</v>
       </c>
       <c r="D63" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E63" s="10" t="s">
-        <v>194</v>
+        <v>87</v>
+      </c>
+      <c r="E63" s="21" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B64" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C64" s="10" t="s">
-        <v>200</v>
+        <v>111</v>
+      </c>
+      <c r="C64" s="21" t="s">
+        <v>199</v>
       </c>
       <c r="D64" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E64" s="10" t="s">
-        <v>196</v>
+        <v>87</v>
+      </c>
+      <c r="E64" s="21" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B65" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C65" s="10" t="s">
-        <v>201</v>
+        <v>111</v>
+      </c>
+      <c r="C65" s="21" t="s">
+        <v>249</v>
       </c>
       <c r="D65" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E65" s="10" t="s">
-        <v>197</v>
+        <v>87</v>
+      </c>
+      <c r="E65" s="21" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B66" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C66" s="10" t="s">
-        <v>202</v>
+        <v>111</v>
+      </c>
+      <c r="C66" s="21" t="s">
+        <v>200</v>
       </c>
       <c r="D66" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E66" s="10" t="s">
-        <v>198</v>
+        <v>87</v>
+      </c>
+      <c r="E66" s="21" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B67" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="C67" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="D67" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="E67" s="10" t="s">
-        <v>199</v>
+        <v>111</v>
+      </c>
+      <c r="C67" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="D67" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E67" s="21" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B68" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C68" s="21" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="D68" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E68" s="21" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B69" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C69" s="21" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D69" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E69" s="21" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B70" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C70" s="21" t="s">
-        <v>207</v>
+        <v>244</v>
       </c>
       <c r="D70" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E70" s="21" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B71" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C71" s="21" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D71" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E71" s="21" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B72" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C72" s="21" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D72" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E72" s="21" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B73" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C73" s="21" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D73" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E73" s="21" t="s">
-        <v>212</v>
+        <v>209</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C74" s="21" t="s">
+        <v>217</v>
+      </c>
+      <c r="D74" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E74" s="21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B75" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C75" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="D75" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E75" s="21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B76" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C76" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="D76" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E76" s="21" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B77" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C77" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="D77" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E77" s="21" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C78" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="D78" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E78" s="21" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C79" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="D79" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E79" s="21" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C80" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="D80" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E80" s="21" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B81" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C81" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="D81" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E81" s="21" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B82" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C82" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="D82" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E82" s="21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B83" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C83" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="D83" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E83" s="21" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B84" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C84" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="D84" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E84" s="21" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B85" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C85" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="D85" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E85" s="21" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B86" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C86" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="D86" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E86" s="21" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B87" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C87" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="D87" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E87" s="21" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B88" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C88" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="D88" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E88" s="21" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B89" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C89" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="D89" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E89" s="21" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed System.out and added few syncs
</commit_message>
<xml_diff>
--- a/TGLAutomation/src/test/resources/testdata/MasterSheet.xlsx
+++ b/TGLAutomation/src/test/resources/testdata/MasterSheet.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="254">
   <si>
     <t>S.N.</t>
   </si>
@@ -780,6 +780,18 @@
   </si>
   <si>
     <t>Tgl_TaxInfoDependentIncome_lbl</t>
+  </si>
+  <si>
+    <t>(//table[@class='verification-table'])[8]//td[1]</t>
+  </si>
+  <si>
+    <t>(//table[@class='verification-table'])[8]//td[2]/tfa-input</t>
+  </si>
+  <si>
+    <t>(//table[@class='verification-table'])[8]//td[3]/tfa-input</t>
+  </si>
+  <si>
+    <t>(//table[@class='verification-table'])[8]//td[4]/tfa-input</t>
   </si>
 </sst>
 </file>
@@ -1700,8 +1712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3190,7 +3202,7 @@
         <v>87</v>
       </c>
       <c r="E86" s="21" t="s">
-        <v>226</v>
+        <v>250</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3207,7 +3219,7 @@
         <v>87</v>
       </c>
       <c r="E87" s="21" t="s">
-        <v>227</v>
+        <v>251</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3224,7 +3236,7 @@
         <v>87</v>
       </c>
       <c r="E88" s="21" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -3241,7 +3253,7 @@
         <v>87</v>
       </c>
       <c r="E89" s="21" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1.Created New test Scripts(TGLPortalUploadTest, TotalAwardSectionTest) 2.Created new testPage(SearchDetailsPageTGL) 3.Updated testPage(SearchPageTGL) 4.Added TGLWebUtil Class(TGLWebUtil)
</commit_message>
<xml_diff>
--- a/TGLAutomation/src/test/resources/testdata/MasterSheet.xlsx
+++ b/TGLAutomation/src/test/resources/testdata/MasterSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Local_Rep\TGL-Automation\tgl-selenium-automation\TGLAutomation\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TGL\TGL_LATEST\tgl-selenium-automation\TGLAutomation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="336">
   <si>
     <t>S.N.</t>
   </si>
@@ -792,6 +792,252 @@
   </si>
   <si>
     <t>(//table[@class='verification-table'])[8]//td[4]/tfa-input</t>
+  </si>
+  <si>
+    <t>errorMessage_Validation_1</t>
+  </si>
+  <si>
+    <t>Only .gif, .jpg, or .pdf files are supported. Please select the appropriate file and try again.</t>
+  </si>
+  <si>
+    <t>errorMessage_Validation_2</t>
+  </si>
+  <si>
+    <t>You must select at least one document type.</t>
+  </si>
+  <si>
+    <t>uploadDocFilePath</t>
+  </si>
+  <si>
+    <t>TGLUploadDocument.docx</t>
+  </si>
+  <si>
+    <t>uploadPDFFilePath</t>
+  </si>
+  <si>
+    <t>TGLUploadDocument.pdf</t>
+  </si>
+  <si>
+    <t>expectedDocumentType</t>
+  </si>
+  <si>
+    <t>TAXFAFSA,ATAXFAFSA,PTAXFAFSA,PINCOME,W2INCOME,PRIVATELOAN,OTHERLOAN,SAVING,CREDITCARDDT,EDUCOST</t>
+  </si>
+  <si>
+    <t>expectedPromptMessage</t>
+  </si>
+  <si>
+    <t>Are you sure you want to update</t>
+  </si>
+  <si>
+    <t>LoanAdjustmentAmount</t>
+  </si>
+  <si>
+    <t>GrantAdjustmentAmount</t>
+  </si>
+  <si>
+    <t>AdjustmentComment</t>
+  </si>
+  <si>
+    <t>QA Testing</t>
+  </si>
+  <si>
+    <t>InValidLoanAdjustmentAmount_1</t>
+  </si>
+  <si>
+    <t>dddd</t>
+  </si>
+  <si>
+    <t>ValidationMessage_1</t>
+  </si>
+  <si>
+    <t>Please enter a number.</t>
+  </si>
+  <si>
+    <t>InValidLoanAdjustmentAmount_2</t>
+  </si>
+  <si>
+    <t>ValidationMessage_2</t>
+  </si>
+  <si>
+    <t>Please round to the nearest whole number.</t>
+  </si>
+  <si>
+    <t>TGL105</t>
+  </si>
+  <si>
+    <t>TGL106</t>
+  </si>
+  <si>
+    <t>Tgl_Search_btn</t>
+  </si>
+  <si>
+    <t>//span[text()='Search']</t>
+  </si>
+  <si>
+    <t>Tgl_FirstRowColumn_TB</t>
+  </si>
+  <si>
+    <t>//tbody[@data-hook='results']/tr[1]/td[1]/a</t>
+  </si>
+  <si>
+    <t>SearchDetailsPage</t>
+  </si>
+  <si>
+    <t>Tgl_UploadTGLDocuments_btn</t>
+  </si>
+  <si>
+    <t>//span[text()='Upload TGL Documents']</t>
+  </si>
+  <si>
+    <t>Tgl_Upload_btn</t>
+  </si>
+  <si>
+    <t>//span[text()='Upload']</t>
+  </si>
+  <si>
+    <t>Tgl_validationErrorMsgWitoutEnterAnyDoc_ST</t>
+  </si>
+  <si>
+    <t>//div[@data-hook='upload-file-error']</t>
+  </si>
+  <si>
+    <t>Tgl_validationErrorMsgDocType_ST</t>
+  </si>
+  <si>
+    <t>//div[@data-hook='doc-type-error']</t>
+  </si>
+  <si>
+    <t>Tgl_ApplicantTaxReturn_CHK</t>
+  </si>
+  <si>
+    <t>//input[@type='checkbox' and @value='ATAXFAFSA']</t>
+  </si>
+  <si>
+    <t>Tgl_UploadedFileIcon_Img</t>
+  </si>
+  <si>
+    <t>//input[@name='uploadedFile']</t>
+  </si>
+  <si>
+    <t>Tgl_DocumentTypeSection_ST</t>
+  </si>
+  <si>
+    <t>//input[@type='checkbox' and @name='docTypes']</t>
+  </si>
+  <si>
+    <t>Tgl_Cancel_btn</t>
+  </si>
+  <si>
+    <t>//button[@data-hook='cancel']//span[text()='Cancel'][1]</t>
+  </si>
+  <si>
+    <t>Tgl_ColTaxReturn_TB</t>
+  </si>
+  <si>
+    <t>//div[@class='support-document']//ancestor::div[@data-hook='applicant-tax-section']//following-sibling::table[@class='documents-table']</t>
+  </si>
+  <si>
+    <t>Tgl_Remove_btn</t>
+  </si>
+  <si>
+    <t>(//span[text()='Yes, remove this document'])[last()]</t>
+  </si>
+  <si>
+    <t>Tgl_DocumentName_ST</t>
+  </si>
+  <si>
+    <t>//td[contains(text(),'TGLUploadDocument')]</t>
+  </si>
+  <si>
+    <t>Tgl_ManuallyAdjust_btn</t>
+  </si>
+  <si>
+    <t>//button[@data-hook='total-award-manually-adjust']</t>
+  </si>
+  <si>
+    <t>Tgl_LoanAdjustment_ED</t>
+  </si>
+  <si>
+    <t>//input[@name='tgl-award-loan-adjustment']</t>
+  </si>
+  <si>
+    <t>Tgl_GrantAdjustment_ED</t>
+  </si>
+  <si>
+    <t>//input[@name='tgl-award-grant-adjustment']</t>
+  </si>
+  <si>
+    <t>Tgl_AdjustmentComment_ED</t>
+  </si>
+  <si>
+    <t>//textarea[@id='tgl-award-adjustment-comment-input']</t>
+  </si>
+  <si>
+    <t>Tgl_AdjustmentSave_btn</t>
+  </si>
+  <si>
+    <t>//button[@data-hook='prompt-adjustment-button']</t>
+  </si>
+  <si>
+    <t>Tgl_AdjustmentCancel_btn</t>
+  </si>
+  <si>
+    <t>//button[@data-hook='cancel-adjustment-button']</t>
+  </si>
+  <si>
+    <t>Tgl_PromptMessage_Msg</t>
+  </si>
+  <si>
+    <t>//div[@class='action-prompt-message']</t>
+  </si>
+  <si>
+    <t>Tgl_CancelNo_btn</t>
+  </si>
+  <si>
+    <t>//button[@data-hook='cancel-button'][1]</t>
+  </si>
+  <si>
+    <t>Tgl_YesUpdateThisAward_btn</t>
+  </si>
+  <si>
+    <t>//span[text()='Yes, update this award']</t>
+  </si>
+  <si>
+    <t>Tgl_AdjustedLoanAmount_ST</t>
+  </si>
+  <si>
+    <t>//tbody//tr[1]//th[@class='tgl-award-breakdown-final']/following-sibling::td[2]</t>
+  </si>
+  <si>
+    <t>Tgl_AdjustedGrantAmount_ST</t>
+  </si>
+  <si>
+    <t>//tbody//tr[3]//th[@class='tgl-award-breakdown-final']/following-sibling::td[2]</t>
+  </si>
+  <si>
+    <t>Tgl_RemoveAdjustment_btn</t>
+  </si>
+  <si>
+    <t>//button[@data-hook='remove-adjustment']</t>
+  </si>
+  <si>
+    <t>Tgl_YesRemoveAdjustment_btn</t>
+  </si>
+  <si>
+    <t>//span[text()='Yes, remove the adjustment']</t>
+  </si>
+  <si>
+    <t>Tgl_ValidationMessage_ST</t>
+  </si>
+  <si>
+    <t>tgl-award-loan-adjustment-validation-message</t>
+  </si>
+  <si>
+    <t>TGL105TestTGLPortalUpload</t>
+  </si>
+  <si>
+    <t>TGL106TestTotalAwardSection</t>
   </si>
 </sst>
 </file>
@@ -877,7 +1123,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -900,12 +1146,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -957,20 +1229,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="36">
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1000,11 +1295,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1017,11 +1312,281 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1374,19 +1939,19 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="23" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1400,10 +1965,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS6"/>
+  <dimension ref="A1:AS8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,9 +1979,9 @@
     <col min="4" max="4" width="11.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="69.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="38.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="36.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="39.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="36.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="34.7109375" style="1" customWidth="1"/>
     <col min="11" max="11" width="38.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="33.7109375" style="1" customWidth="1"/>
@@ -1593,13 +2158,13 @@
       </c>
     </row>
     <row r="2" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="28" t="s">
         <v>106</v>
       </c>
       <c r="D2" s="13" t="s">
@@ -1608,35 +2173,35 @@
       <c r="E2" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="27"/>
       <c r="W2" s="22"/>
       <c r="X2" s="22"/>
       <c r="Y2" s="22"/>
     </row>
     <row r="3" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="28" t="s">
         <v>113</v>
       </c>
       <c r="D3" s="13" t="s">
@@ -1645,15 +2210,31 @@
       <c r="E3" s="12" t="s">
         <v>248</v>
       </c>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="26"/>
+      <c r="U3" s="26"/>
     </row>
     <row r="4" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="28" t="s">
         <v>140</v>
       </c>
       <c r="D4" s="13" t="s">
@@ -1662,15 +2243,31 @@
       <c r="E4" s="12" t="s">
         <v>248</v>
       </c>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="26"/>
+      <c r="M4" s="26"/>
+      <c r="N4" s="26"/>
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
+      <c r="R4" s="26"/>
+      <c r="S4" s="26"/>
+      <c r="T4" s="26"/>
+      <c r="U4" s="26"/>
     </row>
     <row r="5" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="26" t="s">
         <v>215</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="28" t="s">
         <v>213</v>
       </c>
       <c r="D5" s="13" t="s">
@@ -1679,15 +2276,31 @@
       <c r="E5" s="12" t="s">
         <v>248</v>
       </c>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26"/>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+      <c r="U5" s="26"/>
     </row>
     <row r="6" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="25" t="s">
         <v>246</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="26" t="s">
         <v>247</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="28" t="s">
         <v>245</v>
       </c>
       <c r="D6" s="13" t="s">
@@ -1696,10 +2309,144 @@
       <c r="E6" s="12" t="s">
         <v>248</v>
       </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+    </row>
+    <row r="7" spans="1:45" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="35">
+        <v>6</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>277</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>334</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>255</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>256</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="J7" s="26" t="s">
+        <v>258</v>
+      </c>
+      <c r="K7" s="26" t="s">
+        <v>259</v>
+      </c>
+      <c r="L7" s="26" t="s">
+        <v>260</v>
+      </c>
+      <c r="M7" s="26" t="s">
+        <v>261</v>
+      </c>
+      <c r="N7" s="26" t="s">
+        <v>262</v>
+      </c>
+      <c r="O7" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="26"/>
+    </row>
+    <row r="8" spans="1:45" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="35">
+        <v>7</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="F8" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="G8" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>266</v>
+      </c>
+      <c r="I8" s="29">
+        <v>200</v>
+      </c>
+      <c r="J8" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="K8" s="29">
+        <v>100</v>
+      </c>
+      <c r="L8" s="26" t="s">
+        <v>268</v>
+      </c>
+      <c r="M8" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="N8" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="O8" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="P8" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q8" s="26" t="s">
+        <v>273</v>
+      </c>
+      <c r="R8" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="S8" s="29">
+        <v>12.56</v>
+      </c>
+      <c r="T8" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="U8" s="26" t="s">
+        <v>276</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D1048576">
       <formula1>"Y, N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1710,10 +2457,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U89"/>
+  <dimension ref="A1:U116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3256,20 +4003,589 @@
         <v>253</v>
       </c>
     </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B90" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="C90" s="31" t="s">
+        <v>279</v>
+      </c>
+      <c r="D90" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E90" s="31" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B91" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="C91" s="31" t="s">
+        <v>281</v>
+      </c>
+      <c r="D91" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E91" s="31" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B92" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C92" s="31" t="s">
+        <v>284</v>
+      </c>
+      <c r="D92" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E92" s="31" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B93" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C93" s="31" t="s">
+        <v>286</v>
+      </c>
+      <c r="D93" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E93" s="31" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B94" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C94" s="31" t="s">
+        <v>288</v>
+      </c>
+      <c r="D94" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E94" s="31" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B95" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C95" s="31" t="s">
+        <v>290</v>
+      </c>
+      <c r="D95" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E95" s="31" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B96" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C96" s="31" t="s">
+        <v>292</v>
+      </c>
+      <c r="D96" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E96" s="31" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B97" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C97" s="31" t="s">
+        <v>294</v>
+      </c>
+      <c r="D97" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E97" s="31" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B98" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C98" s="31" t="s">
+        <v>296</v>
+      </c>
+      <c r="D98" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E98" s="31" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B99" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C99" s="31" t="s">
+        <v>298</v>
+      </c>
+      <c r="D99" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E99" s="31" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A100" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B100" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="C100" s="31" t="s">
+        <v>300</v>
+      </c>
+      <c r="D100" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E100" s="31" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B101" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="C101" s="33" t="s">
+        <v>302</v>
+      </c>
+      <c r="D101" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E101" s="33" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B102" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="C102" s="33" t="s">
+        <v>304</v>
+      </c>
+      <c r="D102" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E102" s="33" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B103" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C103" s="33" t="s">
+        <v>306</v>
+      </c>
+      <c r="D103" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E103" s="33" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B104" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C104" s="33" t="s">
+        <v>308</v>
+      </c>
+      <c r="D104" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E104" s="33" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B105" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C105" s="33" t="s">
+        <v>310</v>
+      </c>
+      <c r="D105" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E105" s="33" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B106" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C106" s="33" t="s">
+        <v>312</v>
+      </c>
+      <c r="D106" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E106" s="33" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B107" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C107" s="33" t="s">
+        <v>314</v>
+      </c>
+      <c r="D107" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E107" s="21" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B108" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C108" s="33" t="s">
+        <v>316</v>
+      </c>
+      <c r="D108" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E108" s="21" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B109" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C109" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="D109" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E109" s="21" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B110" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C110" s="33" t="s">
+        <v>320</v>
+      </c>
+      <c r="D110" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E110" s="21" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B111" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C111" s="33" t="s">
+        <v>322</v>
+      </c>
+      <c r="D111" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E111" s="21" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A112" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B112" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C112" s="31" t="s">
+        <v>324</v>
+      </c>
+      <c r="D112" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E112" s="21" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B113" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C113" s="31" t="s">
+        <v>326</v>
+      </c>
+      <c r="D113" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E113" s="21" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B114" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C114" s="31" t="s">
+        <v>328</v>
+      </c>
+      <c r="D114" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E114" s="21" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B115" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C115" s="31" t="s">
+        <v>330</v>
+      </c>
+      <c r="D115" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E115" s="21" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B116" s="30" t="s">
+        <v>283</v>
+      </c>
+      <c r="C116" s="31" t="s">
+        <v>332</v>
+      </c>
+      <c r="D116" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E116" s="34" t="s">
+        <v>333</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:A3"/>
-  <conditionalFormatting sqref="D1:D37 D40:D1048576">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+  <conditionalFormatting sqref="D1:D37 D40:D89 D117:D1048576">
+    <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
+      <formula>"id"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
+      <formula>"css"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="36" operator="equal">
       <formula>"xpath"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38:D39">
+    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
+      <formula>"id"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
+      <formula>"css"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
+      <formula>"xpath"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D116 D90:D100">
+    <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
+      <formula>"id"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
+      <formula>"css"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
+      <formula>"xpath"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D101">
+    <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
+      <formula>"id"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="26" operator="equal">
+      <formula>"css"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="27" operator="equal">
+      <formula>"xpath"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D102">
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+      <formula>"id"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+      <formula>"css"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
+      <formula>"xpath"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D103:D105">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+      <formula>"id"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+      <formula>"css"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
+      <formula>"xpath"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D106:D107">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+      <formula>"id"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+      <formula>"css"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+      <formula>"xpath"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D108:D111">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+      <formula>"id"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+      <formula>"css"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+      <formula>"xpath"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D112">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+      <formula>"id"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>"css"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+      <formula>"xpath"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D113">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+      <formula>"id"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>"css"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+      <formula>"xpath"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D114">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"id"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"css"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>"id"</formula>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>"xpath"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D38:D39">
+  <conditionalFormatting sqref="D115">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"id"</formula>
     </cfRule>

</xml_diff>

<commit_message>
committing latest code with code comments
</commit_message>
<xml_diff>
--- a/TGLAutomation/src/test/resources/testdata/MasterSheet.xlsx
+++ b/TGLAutomation/src/test/resources/testdata/MasterSheet.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TGL\TGL_LATEST\tgl-selenium-automation\TGLAutomation\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_Local_Rep\TGL-Automation\tgl-selenium-automation\tgl-selenium-automation\TGLAutomation\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="367">
   <si>
     <t>S.N.</t>
   </si>
@@ -659,9 +659,6 @@
     <t>(//div[@class='document-verification-view'])[5]//td[3]//tfa-input</t>
   </si>
   <si>
-    <t>(//div[@class='document-verification-view'])[5]//td[4]//tfa-input</t>
-  </si>
-  <si>
     <t>Tgl_ApplicantstaxValid_chk</t>
   </si>
   <si>
@@ -692,9 +689,6 @@
     <t>(//table[@class='verification-table'])[5]//td[3]/tfa-input</t>
   </si>
   <si>
-    <t>(//table[@class='verification-table'])[5]//td[4]/tfa-input</t>
-  </si>
-  <si>
     <t>(//table[@class='verification-table'])[6]//td[1]</t>
   </si>
   <si>
@@ -704,9 +698,6 @@
     <t>(//table[@class='verification-table'])[6]//td[3]/tfa-input</t>
   </si>
   <si>
-    <t>(//table[@class='verification-table'])[6]//td[4]/tfa-input</t>
-  </si>
-  <si>
     <t>Tgl_TaxInfoIncome_lbl</t>
   </si>
   <si>
@@ -719,9 +710,6 @@
     <t>(//table[@class='verification-table'])[7]//td[3]/tfa-input</t>
   </si>
   <si>
-    <t>(//table[@class='verification-table'])[7]//td[4]/tfa-input</t>
-  </si>
-  <si>
     <t>Tgl_TaxInforAppTaxReturnedRequired_chk</t>
   </si>
   <si>
@@ -791,9 +779,6 @@
     <t>(//table[@class='verification-table'])[8]//td[3]/tfa-input</t>
   </si>
   <si>
-    <t>(//table[@class='verification-table'])[8]//td[4]/tfa-input</t>
-  </si>
-  <si>
     <t>errorMessage_Validation_1</t>
   </si>
   <si>
@@ -1038,6 +1023,114 @@
   </si>
   <si>
     <t>TGL106TestTotalAwardSection</t>
+  </si>
+  <si>
+    <t>AssetsAndLibilities</t>
+  </si>
+  <si>
+    <t>AdditionalInformation</t>
+  </si>
+  <si>
+    <t>TaxInformation</t>
+  </si>
+  <si>
+    <t>Tgl_TGLStatus_dd</t>
+  </si>
+  <si>
+    <t>#status-input</t>
+  </si>
+  <si>
+    <t>Tgl_SearchPIDValidation_lbl</t>
+  </si>
+  <si>
+    <t>#personid-validation-message</t>
+  </si>
+  <si>
+    <t>(//div[@class='document-verification-view'])[5]//td[4]//tfa-input//textarea</t>
+  </si>
+  <si>
+    <t>(//table[@class='verification-table'])[5]//td[4]/tfa-input//textarea</t>
+  </si>
+  <si>
+    <t>(//table[@class='verification-table'])[6]//td[4]/tfa-input//textarea</t>
+  </si>
+  <si>
+    <t>(//table[@class='verification-table'])[7]//td[4]/tfa-input//textarea</t>
+  </si>
+  <si>
+    <t>(//table[@class='verification-table'])[8]//td[4]/tfa-input//textarea</t>
+  </si>
+  <si>
+    <t>(//object[@component-name='tfa-more-info'])[14]</t>
+  </si>
+  <si>
+    <t>(//div[@data-hook='modal-heading-text'])[20]</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfo_ApplicantTaxReturnHelp_link</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoApplicantTaxReturnHelpModal_lbl</t>
+  </si>
+  <si>
+    <t>(//div[@data-hook='modal-heading-text'])[17]</t>
+  </si>
+  <si>
+    <t>(//object[@component-name='tfa-more-info'])[15]</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoW2Help_link</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfo_HelpModal_lbl</t>
+  </si>
+  <si>
+    <t>(//div[@data-hook='modal-heading-text'])[19]</t>
+  </si>
+  <si>
+    <t>(//object[@component-name='tfa-more-info'])[16]</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoParentsTaxReturnHelp_link</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoParentsTaxReturnHelpModal_lbl</t>
+  </si>
+  <si>
+    <t>(//div[@data-hook='modal-heading-text'])[18]</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoPISHelp_link</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoPISHelpModal_lbl</t>
+  </si>
+  <si>
+    <t>(//object[@component-name='tfa-more-info'])[17]</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfo_ApplicantTaxReturnClose_btn</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoW2HelpMOdalClose_btn</t>
+  </si>
+  <si>
+    <t>((//div[@data-hook='modal-heading-text'])[20])/following-sibling::button</t>
+  </si>
+  <si>
+    <t>(//div[@data-hook='modal-heading-text'])[17]/following-sibling::button</t>
+  </si>
+  <si>
+    <t>(//div[@data-hook='modal-heading-text'])[19]/following-sibling::button</t>
+  </si>
+  <si>
+    <t>(//div[@data-hook='modal-heading-text'])[18]/following-sibling::button</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoParentsTaxReturnHelpModalClose_btn</t>
+  </si>
+  <si>
+    <t>Tgl_TaxInfoPISHelpModalClose_btn</t>
   </si>
 </sst>
 </file>
@@ -1265,7 +1358,34 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="39">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C6500"/>
@@ -1685,23 +1805,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1737,23 +1840,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1908,18 +1994,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="80.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="39.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="3"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
@@ -1956,9 +2033,6 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2171,7 +2245,7 @@
         <v>59</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F2" s="26"/>
       <c r="G2" s="26"/>
@@ -2208,7 +2282,7 @@
         <v>59</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F3" s="26"/>
       <c r="G3" s="26"/>
@@ -2241,7 +2315,7 @@
         <v>59</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F4" s="26"/>
       <c r="G4" s="26"/>
@@ -2262,19 +2336,19 @@
     </row>
     <row r="5" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="B5" s="26" t="s">
         <v>214</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>215</v>
-      </c>
       <c r="C5" s="28" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>59</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F5" s="26"/>
       <c r="G5" s="26"/>
@@ -2295,19 +2369,19 @@
     </row>
     <row r="6" spans="1:45" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>59</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
@@ -2331,46 +2405,46 @@
         <v>6</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>59</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F7" s="26" t="s">
+        <v>249</v>
+      </c>
+      <c r="G7" s="26" t="s">
+        <v>250</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>252</v>
+      </c>
+      <c r="J7" s="26" t="s">
+        <v>253</v>
+      </c>
+      <c r="K7" s="26" t="s">
         <v>254</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="L7" s="26" t="s">
         <v>255</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="M7" s="26" t="s">
         <v>256</v>
       </c>
-      <c r="I7" s="26" t="s">
+      <c r="N7" s="26" t="s">
         <v>257</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="O7" s="26" t="s">
         <v>258</v>
-      </c>
-      <c r="K7" s="26" t="s">
-        <v>259</v>
-      </c>
-      <c r="L7" s="26" t="s">
-        <v>260</v>
-      </c>
-      <c r="M7" s="26" t="s">
-        <v>261</v>
-      </c>
-      <c r="N7" s="26" t="s">
-        <v>262</v>
-      </c>
-      <c r="O7" s="26" t="s">
-        <v>263</v>
       </c>
       <c r="P7" s="26"/>
       <c r="Q7" s="26"/>
@@ -2384,64 +2458,64 @@
         <v>7</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>59</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F8" s="26" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="G8" s="26" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="H8" s="26" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="I8" s="29">
         <v>200</v>
       </c>
       <c r="J8" s="26" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="K8" s="29">
         <v>100</v>
       </c>
       <c r="L8" s="26" t="s">
+        <v>263</v>
+      </c>
+      <c r="M8" s="26" t="s">
+        <v>264</v>
+      </c>
+      <c r="N8" s="26" t="s">
+        <v>265</v>
+      </c>
+      <c r="O8" s="26" t="s">
+        <v>266</v>
+      </c>
+      <c r="P8" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q8" s="26" t="s">
         <v>268</v>
       </c>
-      <c r="M8" s="26" t="s">
+      <c r="R8" s="26" t="s">
         <v>269</v>
-      </c>
-      <c r="N8" s="26" t="s">
-        <v>270</v>
-      </c>
-      <c r="O8" s="26" t="s">
-        <v>271</v>
-      </c>
-      <c r="P8" s="26" t="s">
-        <v>272</v>
-      </c>
-      <c r="Q8" s="26" t="s">
-        <v>273</v>
-      </c>
-      <c r="R8" s="26" t="s">
-        <v>274</v>
       </c>
       <c r="S8" s="29">
         <v>12.56</v>
       </c>
       <c r="T8" s="26" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="U8" s="26" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -2451,25 +2525,25 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U116"/>
+  <dimension ref="A1:U130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="C101" sqref="C101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" style="9" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" style="9" customWidth="1"/>
     <col min="3" max="3" width="56.42578125" style="10" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="67" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="83.28515625" style="10" customWidth="1"/>
     <col min="6" max="21" width="9.140625" style="17"/>
     <col min="22" max="16384" width="9.140625" style="9"/>
   </cols>
@@ -3056,7 +3130,7 @@
         <v>79</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>111</v>
+        <v>331</v>
       </c>
       <c r="C34" s="21" t="s">
         <v>133</v>
@@ -3073,7 +3147,7 @@
         <v>79</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>111</v>
+        <v>331</v>
       </c>
       <c r="C35" s="21" t="s">
         <v>135</v>
@@ -3090,7 +3164,7 @@
         <v>79</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>111</v>
+        <v>331</v>
       </c>
       <c r="C36" s="21" t="s">
         <v>136</v>
@@ -3107,7 +3181,7 @@
         <v>79</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>111</v>
+        <v>331</v>
       </c>
       <c r="C37" s="21" t="s">
         <v>137</v>
@@ -3124,7 +3198,7 @@
         <v>79</v>
       </c>
       <c r="B38" s="20" t="s">
-        <v>111</v>
+        <v>331</v>
       </c>
       <c r="C38" s="21" t="s">
         <v>143</v>
@@ -3141,7 +3215,7 @@
         <v>79</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>111</v>
+        <v>331</v>
       </c>
       <c r="C39" s="21" t="s">
         <v>144</v>
@@ -3158,7 +3232,7 @@
         <v>79</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>111</v>
+        <v>331</v>
       </c>
       <c r="C40" s="21" t="s">
         <v>148</v>
@@ -3175,7 +3249,7 @@
         <v>79</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>111</v>
+        <v>331</v>
       </c>
       <c r="C41" s="21" t="s">
         <v>156</v>
@@ -3192,7 +3266,7 @@
         <v>79</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>111</v>
+        <v>331</v>
       </c>
       <c r="C42" s="21" t="s">
         <v>157</v>
@@ -3209,7 +3283,7 @@
         <v>79</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>111</v>
+        <v>331</v>
       </c>
       <c r="C43" s="21" t="s">
         <v>153</v>
@@ -3226,7 +3300,7 @@
         <v>79</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>111</v>
+        <v>331</v>
       </c>
       <c r="C44" s="21" t="s">
         <v>154</v>
@@ -3243,7 +3317,7 @@
         <v>79</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>111</v>
+        <v>331</v>
       </c>
       <c r="C45" s="21" t="s">
         <v>155</v>
@@ -3260,7 +3334,7 @@
         <v>79</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>111</v>
+        <v>331</v>
       </c>
       <c r="C46" s="21" t="s">
         <v>161</v>
@@ -3277,7 +3351,7 @@
         <v>79</v>
       </c>
       <c r="B47" s="20" t="s">
-        <v>111</v>
+        <v>331</v>
       </c>
       <c r="C47" s="21" t="s">
         <v>164</v>
@@ -3294,7 +3368,7 @@
         <v>79</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>111</v>
+        <v>331</v>
       </c>
       <c r="C48" s="21" t="s">
         <v>165</v>
@@ -3311,7 +3385,7 @@
         <v>79</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>111</v>
+        <v>331</v>
       </c>
       <c r="C49" s="21" t="s">
         <v>166</v>
@@ -3328,7 +3402,7 @@
         <v>79</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>111</v>
+        <v>331</v>
       </c>
       <c r="C50" s="21" t="s">
         <v>167</v>
@@ -3345,7 +3419,7 @@
         <v>79</v>
       </c>
       <c r="B51" s="20" t="s">
-        <v>111</v>
+        <v>331</v>
       </c>
       <c r="C51" s="21" t="s">
         <v>168</v>
@@ -3362,7 +3436,7 @@
         <v>79</v>
       </c>
       <c r="B52" s="20" t="s">
-        <v>111</v>
+        <v>332</v>
       </c>
       <c r="C52" s="21" t="s">
         <v>172</v>
@@ -3379,7 +3453,7 @@
         <v>79</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>111</v>
+        <v>332</v>
       </c>
       <c r="C53" s="21" t="s">
         <v>173</v>
@@ -3396,7 +3470,7 @@
         <v>79</v>
       </c>
       <c r="B54" s="20" t="s">
-        <v>111</v>
+        <v>332</v>
       </c>
       <c r="C54" s="21" t="s">
         <v>174</v>
@@ -3413,7 +3487,7 @@
         <v>79</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>111</v>
+        <v>332</v>
       </c>
       <c r="C55" s="21" t="s">
         <v>175</v>
@@ -3430,7 +3504,7 @@
         <v>79</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>111</v>
+        <v>332</v>
       </c>
       <c r="C56" s="21" t="s">
         <v>176</v>
@@ -3447,7 +3521,7 @@
         <v>79</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>111</v>
+        <v>332</v>
       </c>
       <c r="C57" s="21" t="s">
         <v>177</v>
@@ -3464,7 +3538,7 @@
         <v>79</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>111</v>
+        <v>332</v>
       </c>
       <c r="C58" s="21" t="s">
         <v>184</v>
@@ -3481,7 +3555,7 @@
         <v>79</v>
       </c>
       <c r="B59" s="20" t="s">
-        <v>111</v>
+        <v>332</v>
       </c>
       <c r="C59" s="21" t="s">
         <v>185</v>
@@ -3498,7 +3572,7 @@
         <v>79</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>111</v>
+        <v>332</v>
       </c>
       <c r="C60" s="21" t="s">
         <v>188</v>
@@ -3515,7 +3589,7 @@
         <v>79</v>
       </c>
       <c r="B61" s="20" t="s">
-        <v>111</v>
+        <v>332</v>
       </c>
       <c r="C61" s="21" t="s">
         <v>190</v>
@@ -3532,7 +3606,7 @@
         <v>79</v>
       </c>
       <c r="B62" s="20" t="s">
-        <v>111</v>
+        <v>332</v>
       </c>
       <c r="C62" s="21" t="s">
         <v>192</v>
@@ -3549,7 +3623,7 @@
         <v>79</v>
       </c>
       <c r="B63" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C63" s="21" t="s">
         <v>194</v>
@@ -3566,7 +3640,7 @@
         <v>79</v>
       </c>
       <c r="B64" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C64" s="21" t="s">
         <v>199</v>
@@ -3583,10 +3657,10 @@
         <v>79</v>
       </c>
       <c r="B65" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C65" s="21" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D65" s="20" t="s">
         <v>87</v>
@@ -3600,7 +3674,7 @@
         <v>79</v>
       </c>
       <c r="B66" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C66" s="21" t="s">
         <v>200</v>
@@ -3617,7 +3691,7 @@
         <v>79</v>
       </c>
       <c r="B67" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C67" s="21" t="s">
         <v>201</v>
@@ -3634,7 +3708,7 @@
         <v>79</v>
       </c>
       <c r="B68" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C68" s="21" t="s">
         <v>205</v>
@@ -3651,7 +3725,7 @@
         <v>79</v>
       </c>
       <c r="B69" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C69" s="21" t="s">
         <v>206</v>
@@ -3668,10 +3742,10 @@
         <v>79</v>
       </c>
       <c r="B70" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C70" s="21" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D70" s="20" t="s">
         <v>87</v>
@@ -3685,10 +3759,10 @@
         <v>79</v>
       </c>
       <c r="B71" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C71" s="21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D71" s="20" t="s">
         <v>87</v>
@@ -3702,10 +3776,10 @@
         <v>79</v>
       </c>
       <c r="B72" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C72" s="21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D72" s="20" t="s">
         <v>87</v>
@@ -3719,16 +3793,16 @@
         <v>79</v>
       </c>
       <c r="B73" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C73" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D73" s="20" t="s">
         <v>87</v>
       </c>
       <c r="E73" s="21" t="s">
-        <v>209</v>
+        <v>338</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3736,16 +3810,16 @@
         <v>79</v>
       </c>
       <c r="B74" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C74" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D74" s="20" t="s">
         <v>87</v>
       </c>
       <c r="E74" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3753,16 +3827,16 @@
         <v>79</v>
       </c>
       <c r="B75" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C75" s="21" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="D75" s="20" t="s">
         <v>87</v>
       </c>
       <c r="E75" s="21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3770,16 +3844,16 @@
         <v>79</v>
       </c>
       <c r="B76" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C76" s="21" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D76" s="20" t="s">
         <v>87</v>
       </c>
       <c r="E76" s="21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3787,16 +3861,16 @@
         <v>79</v>
       </c>
       <c r="B77" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C77" s="21" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D77" s="20" t="s">
         <v>87</v>
       </c>
       <c r="E77" s="21" t="s">
-        <v>220</v>
+        <v>339</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3804,16 +3878,16 @@
         <v>79</v>
       </c>
       <c r="B78" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C78" s="21" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D78" s="20" t="s">
         <v>87</v>
       </c>
       <c r="E78" s="21" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3821,16 +3895,16 @@
         <v>79</v>
       </c>
       <c r="B79" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C79" s="21" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D79" s="20" t="s">
         <v>87</v>
       </c>
       <c r="E79" s="21" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -3838,16 +3912,16 @@
         <v>79</v>
       </c>
       <c r="B80" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C80" s="21" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="D80" s="20" t="s">
         <v>87</v>
       </c>
       <c r="E80" s="21" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -3855,16 +3929,16 @@
         <v>79</v>
       </c>
       <c r="B81" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C81" s="21" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D81" s="20" t="s">
         <v>87</v>
       </c>
       <c r="E81" s="21" t="s">
-        <v>224</v>
+        <v>340</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -3872,16 +3946,16 @@
         <v>79</v>
       </c>
       <c r="B82" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C82" s="21" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D82" s="20" t="s">
         <v>87</v>
       </c>
       <c r="E82" s="21" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -3889,16 +3963,16 @@
         <v>79</v>
       </c>
       <c r="B83" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C83" s="21" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D83" s="20" t="s">
         <v>87</v>
       </c>
       <c r="E83" s="21" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -3906,16 +3980,16 @@
         <v>79</v>
       </c>
       <c r="B84" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C84" s="21" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D84" s="20" t="s">
         <v>87</v>
       </c>
       <c r="E84" s="21" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -3923,16 +3997,16 @@
         <v>79</v>
       </c>
       <c r="B85" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C85" s="21" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D85" s="20" t="s">
         <v>87</v>
       </c>
       <c r="E85" s="21" t="s">
-        <v>229</v>
+        <v>341</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -3940,16 +4014,16 @@
         <v>79</v>
       </c>
       <c r="B86" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C86" s="21" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D86" s="20" t="s">
         <v>87</v>
       </c>
       <c r="E86" s="21" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -3957,16 +4031,16 @@
         <v>79</v>
       </c>
       <c r="B87" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C87" s="21" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D87" s="20" t="s">
         <v>87</v>
       </c>
       <c r="E87" s="21" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -3974,16 +4048,16 @@
         <v>79</v>
       </c>
       <c r="B88" s="20" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="C88" s="21" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D88" s="20" t="s">
         <v>87</v>
       </c>
       <c r="E88" s="21" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -3991,480 +4065,729 @@
         <v>79</v>
       </c>
       <c r="B89" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="C89" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="D89" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E89" s="21" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B90" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="C90" s="21" t="s">
+        <v>345</v>
+      </c>
+      <c r="D90" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E90" s="21" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B91" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="C91" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="D91" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E91" s="21" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B92" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="C92" s="21" t="s">
+        <v>349</v>
+      </c>
+      <c r="D92" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E92" s="21" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B93" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="C93" s="21" t="s">
+        <v>350</v>
+      </c>
+      <c r="D93" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E93" s="21" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B94" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="C94" s="21" t="s">
+        <v>353</v>
+      </c>
+      <c r="D94" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E94" s="21" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B95" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="C95" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="D95" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E95" s="21" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B96" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="C96" s="21" t="s">
+        <v>356</v>
+      </c>
+      <c r="D96" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E96" s="21" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B97" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="C97" s="21" t="s">
+        <v>357</v>
+      </c>
+      <c r="D97" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E97" s="21" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B98" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="C98" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="D98" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E98" s="21" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B99" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="C99" s="21" t="s">
+        <v>360</v>
+      </c>
+      <c r="D99" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E99" s="21" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B100" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="C100" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="D100" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E100" s="21" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B101" s="20" t="s">
+        <v>333</v>
+      </c>
+      <c r="C101" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="D101" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="E101" s="21" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B102" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="C89" s="21" t="s">
-        <v>243</v>
-      </c>
-      <c r="D89" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="E89" s="21" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B90" s="30" t="s">
+      <c r="C102" s="31" t="s">
+        <v>274</v>
+      </c>
+      <c r="D102" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E102" s="31" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B103" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="C90" s="31" t="s">
+      <c r="C103" s="31" t="s">
+        <v>276</v>
+      </c>
+      <c r="D103" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E103" s="31" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B104" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C104" s="31" t="s">
         <v>279</v>
       </c>
-      <c r="D90" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E90" s="31" t="s">
+      <c r="D104" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E104" s="31" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B91" s="30" t="s">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B105" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C105" s="31" t="s">
+        <v>281</v>
+      </c>
+      <c r="D105" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E105" s="31" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B106" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C106" s="31" t="s">
+        <v>283</v>
+      </c>
+      <c r="D106" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E106" s="31" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B107" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C107" s="31" t="s">
+        <v>285</v>
+      </c>
+      <c r="D107" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E107" s="31" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B108" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C108" s="31" t="s">
+        <v>287</v>
+      </c>
+      <c r="D108" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E108" s="31" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B109" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C109" s="31" t="s">
+        <v>289</v>
+      </c>
+      <c r="D109" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E109" s="31" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B110" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C110" s="31" t="s">
+        <v>291</v>
+      </c>
+      <c r="D110" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E110" s="31" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B111" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C111" s="31" t="s">
+        <v>293</v>
+      </c>
+      <c r="D111" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E111" s="31" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A112" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B112" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="C91" s="31" t="s">
-        <v>281</v>
-      </c>
-      <c r="D91" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E91" s="31" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B92" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C92" s="31" t="s">
-        <v>284</v>
-      </c>
-      <c r="D92" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E92" s="31" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B93" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C93" s="31" t="s">
-        <v>286</v>
-      </c>
-      <c r="D93" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E93" s="31" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B94" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C94" s="31" t="s">
-        <v>288</v>
-      </c>
-      <c r="D94" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E94" s="31" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B95" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C95" s="31" t="s">
-        <v>290</v>
-      </c>
-      <c r="D95" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E95" s="31" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B96" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C96" s="31" t="s">
-        <v>292</v>
-      </c>
-      <c r="D96" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E96" s="31" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B97" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C97" s="31" t="s">
-        <v>294</v>
-      </c>
-      <c r="D97" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E97" s="31" t="s">
+      <c r="C112" s="31" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B98" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C98" s="31" t="s">
+      <c r="D112" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E112" s="31" t="s">
         <v>296</v>
       </c>
-      <c r="D98" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E98" s="31" t="s">
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B113" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="C113" s="33" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B99" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C99" s="31" t="s">
+      <c r="D113" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E113" s="33" t="s">
         <v>298</v>
       </c>
-      <c r="D99" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E99" s="31" t="s">
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B114" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="C114" s="33" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A100" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B100" s="30" t="s">
+      <c r="D114" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E114" s="33" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B115" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C115" s="33" t="s">
+        <v>301</v>
+      </c>
+      <c r="D115" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E115" s="33" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B116" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C116" s="33" t="s">
+        <v>303</v>
+      </c>
+      <c r="D116" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E116" s="33" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B117" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C117" s="33" t="s">
+        <v>305</v>
+      </c>
+      <c r="D117" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E117" s="33" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B118" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C118" s="33" t="s">
+        <v>307</v>
+      </c>
+      <c r="D118" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E118" s="33" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B119" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C119" s="33" t="s">
+        <v>309</v>
+      </c>
+      <c r="D119" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E119" s="21" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B120" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C120" s="33" t="s">
+        <v>311</v>
+      </c>
+      <c r="D120" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E120" s="21" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B121" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C121" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="D121" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E121" s="21" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B122" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C122" s="33" t="s">
+        <v>315</v>
+      </c>
+      <c r="D122" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E122" s="21" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B123" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C123" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="D123" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E123" s="21" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B124" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C124" s="31" t="s">
+        <v>319</v>
+      </c>
+      <c r="D124" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E124" s="21" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B125" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C125" s="31" t="s">
+        <v>321</v>
+      </c>
+      <c r="D125" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E125" s="21" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B126" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C126" s="31" t="s">
+        <v>323</v>
+      </c>
+      <c r="D126" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E126" s="21" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B127" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C127" s="31" t="s">
+        <v>325</v>
+      </c>
+      <c r="D127" s="30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E127" s="21" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B128" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="C128" s="31" t="s">
+        <v>327</v>
+      </c>
+      <c r="D128" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E128" s="34" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B129" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="C100" s="31" t="s">
-        <v>300</v>
-      </c>
-      <c r="D100" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E100" s="31" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="B101" s="32" t="s">
+      <c r="C129" s="21" t="s">
+        <v>334</v>
+      </c>
+      <c r="D129" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E129" s="21" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B130" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="C101" s="33" t="s">
-        <v>302</v>
-      </c>
-      <c r="D101" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="E101" s="33" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="B102" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="C102" s="33" t="s">
-        <v>304</v>
-      </c>
-      <c r="D102" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="E102" s="33" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="B103" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C103" s="33" t="s">
-        <v>306</v>
-      </c>
-      <c r="D103" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="E103" s="33" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="B104" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C104" s="33" t="s">
-        <v>308</v>
-      </c>
-      <c r="D104" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="E104" s="33" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="B105" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C105" s="33" t="s">
-        <v>310</v>
-      </c>
-      <c r="D105" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="E105" s="33" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="B106" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C106" s="33" t="s">
-        <v>312</v>
-      </c>
-      <c r="D106" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="E106" s="33" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="B107" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C107" s="33" t="s">
-        <v>314</v>
-      </c>
-      <c r="D107" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="E107" s="21" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="B108" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C108" s="33" t="s">
-        <v>316</v>
-      </c>
-      <c r="D108" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="E108" s="21" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="B109" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C109" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="D109" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="E109" s="21" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="B110" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C110" s="33" t="s">
-        <v>320</v>
-      </c>
-      <c r="D110" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="E110" s="21" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="B111" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C111" s="33" t="s">
-        <v>322</v>
-      </c>
-      <c r="D111" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="E111" s="21" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A112" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B112" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C112" s="31" t="s">
-        <v>324</v>
-      </c>
-      <c r="D112" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E112" s="21" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B113" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C113" s="31" t="s">
-        <v>326</v>
-      </c>
-      <c r="D113" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E113" s="21" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B114" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C114" s="31" t="s">
-        <v>328</v>
-      </c>
-      <c r="D114" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E114" s="21" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B115" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C115" s="31" t="s">
-        <v>330</v>
-      </c>
-      <c r="D115" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="E115" s="21" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="B116" s="30" t="s">
-        <v>283</v>
-      </c>
-      <c r="C116" s="31" t="s">
-        <v>332</v>
-      </c>
-      <c r="D116" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E116" s="34" t="s">
-        <v>333</v>
+      <c r="C130" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="D130" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E130" s="10" t="s">
+        <v>337</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:A3"/>
-  <conditionalFormatting sqref="D1:D37 D40:D89 D117:D1048576">
+  <conditionalFormatting sqref="D1:D37 D131:D1048576 D40:D101">
+    <cfRule type="cellIs" dxfId="38" priority="37" operator="equal">
+      <formula>"id"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="38" operator="equal">
+      <formula>"css"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="39" operator="equal">
+      <formula>"xpath"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38:D39">
     <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
       <formula>"id"</formula>
     </cfRule>
@@ -4475,7 +4798,7 @@
       <formula>"xpath"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D38:D39">
+  <conditionalFormatting sqref="D128 D102:D112">
     <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
       <formula>"id"</formula>
     </cfRule>
@@ -4486,7 +4809,7 @@
       <formula>"xpath"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D116 D90:D100">
+  <conditionalFormatting sqref="D113">
     <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
       <formula>"id"</formula>
     </cfRule>
@@ -4497,7 +4820,7 @@
       <formula>"xpath"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D101">
+  <conditionalFormatting sqref="D114">
     <cfRule type="cellIs" dxfId="26" priority="25" operator="equal">
       <formula>"id"</formula>
     </cfRule>
@@ -4508,7 +4831,7 @@
       <formula>"xpath"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D102">
+  <conditionalFormatting sqref="D115:D117">
     <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
       <formula>"id"</formula>
     </cfRule>
@@ -4519,7 +4842,7 @@
       <formula>"xpath"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D103:D105">
+  <conditionalFormatting sqref="D118:D119">
     <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
       <formula>"id"</formula>
     </cfRule>
@@ -4530,7 +4853,7 @@
       <formula>"xpath"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D106:D107">
+  <conditionalFormatting sqref="D120:D123">
     <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
       <formula>"id"</formula>
     </cfRule>
@@ -4541,7 +4864,7 @@
       <formula>"xpath"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D108:D111">
+  <conditionalFormatting sqref="D124">
     <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
       <formula>"id"</formula>
     </cfRule>
@@ -4552,7 +4875,7 @@
       <formula>"xpath"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D112">
+  <conditionalFormatting sqref="D125">
     <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"id"</formula>
     </cfRule>
@@ -4563,7 +4886,7 @@
       <formula>"xpath"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D113">
+  <conditionalFormatting sqref="D126">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>"id"</formula>
     </cfRule>
@@ -4574,7 +4897,7 @@
       <formula>"xpath"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D114">
+  <conditionalFormatting sqref="D127">
     <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"id"</formula>
     </cfRule>
@@ -4585,7 +4908,7 @@
       <formula>"xpath"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D115">
+  <conditionalFormatting sqref="D129:D130">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"id"</formula>
     </cfRule>
@@ -4602,6 +4925,5 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>